<commit_message>
-atualizacao geral do app
</commit_message>
<xml_diff>
--- a/app/src/main/assets/xls/planilha_full.xlsx
+++ b/app/src/main/assets/xls/planilha_full.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresilva/Library/Mobile Documents/com~apple~CloudDocs/Projetos_Android/Controle_Material/app/src/main/assets/xls/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresilva/Android Apps/ipev carga/app/src/main/assets/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF5E45A-B576-AB49-8C34-38898103A3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7919E3A3-48A3-5949-A6D3-5DAAC55C7F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="500" windowWidth="28700" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="28700" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pag1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'pag1'!$B$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'pag1'!$B$4:$G$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,15 +43,9 @@
     <t>Setor</t>
   </si>
   <si>
-    <t>Estado</t>
-  </si>
-  <si>
     <t>Descrição do item</t>
   </si>
   <si>
-    <t>Observação</t>
-  </si>
-  <si>
     <t>Sala</t>
   </si>
   <si>
@@ -62,6 +56,12 @@
   </si>
   <si>
     <t>SN</t>
+  </si>
+  <si>
+    <t>Observacão</t>
+  </si>
+  <si>
+    <t>MATERIAL CARGA  -  IPEV</t>
   </si>
 </sst>
 </file>
@@ -85,8 +85,8 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,7 +106,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -157,11 +157,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -175,10 +212,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -399,53 +442,68 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.5" style="6"/>
-    <col min="5" max="5" width="28.1640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="22.5" style="6" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="6" customWidth="1"/>
-    <col min="8" max="8" width="56.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="60" style="5" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:8" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:H1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B4:G4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.38" bottom="0.4" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>